<commit_message>
commit 3 - registra bien los contratistas
</commit_message>
<xml_diff>
--- a/otros archivos/correos.xlsx
+++ b/otros archivos/correos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pipe\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crudfetch\otros archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF36F9C3-EB13-40C0-B716-C154F0F3727C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF1F6E6-A095-4017-A474-AF5D89F7C77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{33F9C109-9A92-4E8F-906E-D533E0E0E1B7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t xml:space="preserve">rut </t>
   </si>
@@ -49,9 +49,6 @@
     <t>hora correo</t>
   </si>
   <si>
-    <t xml:space="preserve">fecha correo </t>
-  </si>
-  <si>
     <t>empresa</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>ricardo</t>
   </si>
   <si>
-    <t>santibañez</t>
-  </si>
-  <si>
     <t>7108182-6</t>
   </si>
   <si>
@@ -173,6 +167,15 @@
   </si>
   <si>
     <t>vazquez</t>
+  </si>
+  <si>
+    <t>true o false</t>
+  </si>
+  <si>
+    <t>santibañez solabarrieta</t>
+  </si>
+  <si>
+    <t>autorizado</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +209,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,12 +237,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,24 +559,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF88D5E-B7C6-4748-9FC4-9A8296AB8C35}">
-  <dimension ref="B1:K8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -567,48 +590,45 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1">
-        <v>44646</v>
       </c>
       <c r="I2" s="2">
         <v>0.90833333333333333</v>
@@ -617,96 +637,89 @@
         <v>44649</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1">
-        <v>44645</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1">
-        <v>44645</v>
+        <v>21</v>
       </c>
       <c r="I4" s="2">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1">
-        <v>44645</v>
+        <v>21</v>
       </c>
       <c r="I5" s="2">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1">
-        <v>44646</v>
       </c>
       <c r="I6" s="2">
         <v>0.87083333333333324</v>
@@ -714,51 +727,42 @@
       <c r="J6" s="1">
         <v>44647</v>
       </c>
-      <c r="K6" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="1">
-        <v>44646</v>
       </c>
       <c r="I7" s="2">
         <v>0.3756944444444445</v>
       </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="1">
-        <v>44646</v>
       </c>
       <c r="I8" s="2">
         <v>0.33611111111111108</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -786,15 +790,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -802,10 +806,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -813,10 +817,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>20</v>

</xml_diff>